<commit_message>
filled in the training/testing column in the sheet
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="23250" windowHeight="13170"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$37</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t>Image name</t>
   </si>
@@ -522,14 +525,14 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,6 +583,9 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -594,6 +600,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -608,6 +617,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
@@ -639,6 +651,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -653,6 +668,9 @@
       <c r="D8">
         <v>0</v>
       </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -667,6 +685,9 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -681,6 +702,9 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -695,8 +719,11 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75">
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -713,7 +740,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -725,6 +752,9 @@
       </c>
       <c r="D14">
         <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -740,6 +770,9 @@
       <c r="D15">
         <v>0</v>
       </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
@@ -754,6 +787,9 @@
       <c r="D16">
         <v>0</v>
       </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
@@ -768,8 +804,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75">
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
@@ -786,7 +825,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75">
+    <row r="20" spans="1:6" ht="15">
       <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
@@ -803,7 +842,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75">
+    <row r="21" spans="1:6" ht="15">
       <c r="A21" s="6" t="s">
         <v>35</v>
       </c>
@@ -820,7 +859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75">
+    <row r="22" spans="1:6" ht="15">
       <c r="A22" s="6" t="s">
         <v>36</v>
       </c>
@@ -837,7 +876,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75">
+    <row r="23" spans="1:6" ht="15">
       <c r="A23" s="6" t="s">
         <v>37</v>
       </c>
@@ -854,7 +893,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75">
+    <row r="24" spans="1:6" ht="15">
       <c r="A24" s="6" t="s">
         <v>38</v>
       </c>
@@ -871,7 +910,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75">
+    <row r="26" spans="1:6" ht="15">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -888,7 +927,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75">
+    <row r="27" spans="1:6" ht="15">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -900,6 +939,9 @@
       </c>
       <c r="D27" s="5">
         <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -915,6 +957,9 @@
       <c r="D28">
         <v>0</v>
       </c>
+      <c r="F28" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
@@ -929,6 +974,9 @@
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="F29" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
@@ -943,8 +991,11 @@
       <c r="D30">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75">
+      <c r="F30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -961,7 +1012,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75">
+    <row r="33" spans="1:6" ht="15">
       <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
@@ -978,7 +1029,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75">
+    <row r="34" spans="1:6" ht="15">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -995,7 +1046,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75">
+    <row r="35" spans="1:6" ht="15">
       <c r="A35" s="6" t="s">
         <v>30</v>
       </c>
@@ -1012,7 +1063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75">
+    <row r="36" spans="1:6" ht="15">
       <c r="A36" s="6" t="s">
         <v>31</v>
       </c>
@@ -1029,7 +1080,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75">
+    <row r="37" spans="1:6" ht="15">
       <c r="A37" s="6" t="s">
         <v>32</v>
       </c>
@@ -1058,7 +1109,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1070,7 +1121,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>